<commit_message>
Added ability to refer to standards by multiple names.
</commit_message>
<xml_diff>
--- a/data-raw/isotope.standards.raggedarray.xlsx
+++ b/data-raw/isotope.standards.raggedarray.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwh/Dropbox/Documents/RPackages/HEEL/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE4F8AB-99D1-A248-94C6-D6A3FD388541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F47677-E081-D14F-A554-17509277AB40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="5460" windowWidth="33600" windowHeight="17440" xr2:uid="{BC01E585-F9B4-1C40-8E70-833A08362EF2}"/>
+    <workbookView xWindow="0" yWindow="1960" windowWidth="33600" windowHeight="17440" xr2:uid="{BC01E585-F9B4-1C40-8E70-833A08362EF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -254,6 +254,45 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Cholestane</t>
+  </si>
+  <si>
+    <t>IAEAS1</t>
+  </si>
+  <si>
+    <t>FA_16_1n7</t>
+  </si>
+  <si>
+    <t>FA_18_1n6</t>
+  </si>
+  <si>
+    <t>FA_18_2n6</t>
+  </si>
+  <si>
+    <t>FA_18_3n3</t>
+  </si>
+  <si>
+    <t>FA_20_4n6</t>
+  </si>
+  <si>
+    <t>FA_22_6n3</t>
+  </si>
+  <si>
+    <t>FA_C13_0</t>
+  </si>
+  <si>
+    <t>FA_C13_0ME</t>
+  </si>
+  <si>
+    <t>FA_C15_0</t>
+  </si>
+  <si>
+    <t>FA_C19_0</t>
+  </si>
+  <si>
+    <t>FA_C19_0ME</t>
   </si>
 </sst>
 </file>
@@ -630,7 +669,7 @@
   <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -654,398 +693,398 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1.0862318908081489E-2</v>
+        <v>63</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.0000000000000001E-6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1.0883024892583373E-2</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5">
+        <v>75.52</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.0861910608780719E-2</v>
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="5">
+        <v>23.14</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="4">
-        <v>1.082672140286065E-2</v>
+        <v>3.6764705882352941E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.1035326345452501E-2</v>
+        <v>63</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.0529237599999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.1048172792017646E-2</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3">
+        <v>40.442999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1.098155292505521E-2</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.9189999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>36</v>
+      </c>
+      <c r="C9" s="5">
+        <v>15.721</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5">
-        <v>75.52</v>
+        <v>35.915999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="5">
-        <v>23.14</v>
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.096333486069026E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="4">
-        <v>3.6764705882352941E-3</v>
+        <v>3.6720203602941177E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="8">
-        <v>2.0529237599999999E-3</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3">
+        <v>36.094999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3">
-        <v>40.442999999999998</v>
+        <v>5.3010000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3">
-        <v>7.9189999999999996</v>
+        <v>36</v>
+      </c>
+      <c r="C15" s="5">
+        <v>10.523</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5">
-        <v>15.721</v>
+        <v>48.081000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5">
-        <v>35.915999999999997</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.0936803679455593E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="4">
-        <v>1.096333486069026E-2</v>
+        <v>3.63996375E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="4">
-        <v>3.6720203602941177E-3</v>
+        <v>59</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.9650759479999998E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="3">
-        <v>36.094999999999999</v>
+        <v>59</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1.313259288E-4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="3">
-        <v>5.3010000000000002</v>
+        <v>76</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.098155292505521E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="5">
-        <v>10.523</v>
+        <v>37</v>
+      </c>
+      <c r="C22" s="3">
+        <v>51.9</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5">
-        <v>48.081000000000003</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="4">
-        <v>1.0936803679455593E-2</v>
+        <v>1.1072826601439999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="4">
-        <v>3.63996375E-3</v>
+        <v>3.6812500000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="8">
-        <v>1.9650759479999998E-3</v>
+        <v>78</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1.0862318908081489E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="8">
-        <v>1.313259288E-4</v>
+        <v>79</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.0883024892583373E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="4">
-        <v>1.0838472529532678E-2</v>
+        <v>1.0861910608780719E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="4">
-        <v>1.0837054773937637E-2</v>
+        <v>1.082672140286065E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="4">
-        <v>1.0852858707195915E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>1.1035326345452501E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="4">
-        <v>1.0846449347306907E-2</v>
+        <v>1.1048172792017646E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C32" s="4">
-        <v>1.0846935460494134E-2</v>
+        <v>1.0838472529532678E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C33" s="4">
-        <v>1.0844979268581318E-2</v>
+        <v>1.0837054773937637E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="3">
-        <v>51.9</v>
+        <v>86</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1.0852858707195915E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="5">
-        <v>8.8000000000000007</v>
+        <v>87</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1.0846449347306907E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C36" s="4">
-        <v>1.1072826601439999E-2</v>
+        <v>1.0846935460494134E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C37" s="4">
-        <v>3.6812500000000001E-3</v>
+        <v>1.0844979268581318E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1336,7 +1375,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>66</v>
@@ -2622,9 +2661,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C615">
-    <sortCondition ref="A2:A615"/>
-    <sortCondition ref="B2:B615"/>
+  <sortState ref="A2:C180">
+    <sortCondition ref="A2:A180"/>
+    <sortCondition ref="B2:B180"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>